<commit_message>
Lotrle | Nowe Animacje
</commit_message>
<xml_diff>
--- a/Ardeno/Helpers/Quizz.xlsx
+++ b/Ardeno/Helpers/Quizz.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\Repozytorium GIT\Ardeno\Ardeno\Helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F06C37-E696-4EF0-8275-BB1D82F7DE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95749D48-244C-4AB7-A3F1-A54BE439026D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{53000B35-D2F7-4182-A57B-4B39AAB586BB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="183">
   <si>
     <t>Id</t>
   </si>
@@ -419,6 +419,171 @@
   </si>
   <si>
     <t>Tom Bombadil</t>
+  </si>
+  <si>
+    <t>Jak nazywał się kucyk Sama?</t>
+  </si>
+  <si>
+    <t>Nie miał kucyka</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Brill</t>
+  </si>
+  <si>
+    <t>Billi</t>
+  </si>
+  <si>
+    <t>Erebor to inaczej?</t>
+  </si>
+  <si>
+    <t>Samotna Góra</t>
+  </si>
+  <si>
+    <t>Khazad- dum</t>
+  </si>
+  <si>
+    <t>Moria</t>
+  </si>
+  <si>
+    <t>Belegost</t>
+  </si>
+  <si>
+    <t>Ile było Istarich?</t>
+  </si>
+  <si>
+    <t>Jak zginął Theoden?</t>
+  </si>
+  <si>
+    <t>Został przygnieciony swoim koniem</t>
+  </si>
+  <si>
+    <t>Został przeszyty włócznią</t>
+  </si>
+  <si>
+    <t>Zabił go Nazhul</t>
+  </si>
+  <si>
+    <t>Zabił go Saruman</t>
+  </si>
+  <si>
+    <t>Jak brzmi prawdziwe imię Gandalfa?</t>
+  </si>
+  <si>
+    <t>Olorin</t>
+  </si>
+  <si>
+    <t>Iluvatar</t>
+  </si>
+  <si>
+    <t>Curunir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Czy którykolwiek kransolud postawił swoją stopę w Amanie? </t>
+  </si>
+  <si>
+    <t>Żaden, żyły tylko w Śródziemiu</t>
+  </si>
+  <si>
+    <t>Tak, tylko jeden</t>
+  </si>
+  <si>
+    <t>Tak, było to plemie Ognistobrodych</t>
+  </si>
+  <si>
+    <t>Wiele plemion mieszkało w Amanie w Erze Drzew</t>
+  </si>
+  <si>
+    <t>Legolas, Gimli, Aragorn</t>
+  </si>
+  <si>
+    <t>Kto wchodził w skład Szarej Drużyny?</t>
+  </si>
+  <si>
+    <t>Trzydziestu jeden Dunedainów, Gimli, Legolas oraz synowie Elronda</t>
+  </si>
+  <si>
+    <t>Eomer, Gandalf, Gimli, Legolas i Aragorn</t>
+  </si>
+  <si>
+    <t>Gandalf, trzydziestu jeden Dunedainów, Gimli i Legolas</t>
+  </si>
+  <si>
+    <t>Jak został nazwany Balrog z Morii?</t>
+  </si>
+  <si>
+    <t>Zguba Durina</t>
+  </si>
+  <si>
+    <t>Gothmog</t>
+  </si>
+  <si>
+    <t>Pallando</t>
+  </si>
+  <si>
+    <t>Tar Goroth</t>
+  </si>
+  <si>
+    <t>Język elfów to:</t>
+  </si>
+  <si>
+    <t>Quendi</t>
+  </si>
+  <si>
+    <t>Quenya</t>
+  </si>
+  <si>
+    <t>Khazdul</t>
+  </si>
+  <si>
+    <t>Falathrin</t>
+  </si>
+  <si>
+    <t>Którzy członkowie kompanii Thorina zginęli?</t>
+  </si>
+  <si>
+    <t>Kili, Fili, Thorin</t>
+  </si>
+  <si>
+    <t>Kili, Bombur, Thorin</t>
+  </si>
+  <si>
+    <t>Thorin, Nori, Kili</t>
+  </si>
+  <si>
+    <t>Fili, Kili, Thorin, Bombur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Easy </t>
+  </si>
+  <si>
+    <t>Rivendell to inaczej:</t>
+  </si>
+  <si>
+    <t>Imladris</t>
+  </si>
+  <si>
+    <t>Lorien</t>
+  </si>
+  <si>
+    <t>Fornost</t>
+  </si>
+  <si>
+    <t>Angmar</t>
+  </si>
+  <si>
+    <t>Kto zabił pierwszego smoka?</t>
+  </si>
+  <si>
+    <t>Beleg</t>
+  </si>
+  <si>
+    <t>Gil-Galad</t>
+  </si>
+  <si>
+    <t>Ile znanych jest związków Elfki i Człowieka?</t>
   </si>
 </sst>
 </file>
@@ -787,10 +952,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C17D72F5-F4FD-45E1-8EE5-C8B9682BAF54}">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -798,10 +965,10 @@
     <col min="2" max="2" width="8.77734375" customWidth="1"/>
     <col min="3" max="3" width="63.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="44" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="56.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1638,6 +1805,846 @@
         <v>0</v>
       </c>
     </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" t="s">
+        <v>128</v>
+      </c>
+      <c r="D29" t="s">
+        <v>129</v>
+      </c>
+      <c r="E29" t="s">
+        <v>130</v>
+      </c>
+      <c r="F29" t="s">
+        <v>132</v>
+      </c>
+      <c r="G29" t="s">
+        <v>131</v>
+      </c>
+      <c r="H29" t="str">
+        <f>F29</f>
+        <v>Billi</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>133</v>
+      </c>
+      <c r="D30" t="s">
+        <v>136</v>
+      </c>
+      <c r="E30" t="s">
+        <v>137</v>
+      </c>
+      <c r="F30" t="s">
+        <v>135</v>
+      </c>
+      <c r="G30" t="s">
+        <v>134</v>
+      </c>
+      <c r="H30" t="str">
+        <f>G30</f>
+        <v>Samotna Góra</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" t="s">
+        <v>138</v>
+      </c>
+      <c r="D31">
+        <v>5</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+      <c r="F31">
+        <v>3</v>
+      </c>
+      <c r="G31">
+        <v>12</v>
+      </c>
+      <c r="H31">
+        <f>D31</f>
+        <v>5</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" t="s">
+        <v>139</v>
+      </c>
+      <c r="D32" t="s">
+        <v>143</v>
+      </c>
+      <c r="E32" t="s">
+        <v>140</v>
+      </c>
+      <c r="F32" t="s">
+        <v>141</v>
+      </c>
+      <c r="G32" t="s">
+        <v>142</v>
+      </c>
+      <c r="H32" t="str">
+        <f>E32</f>
+        <v>Został przygnieciony swoim koniem</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" t="s">
+        <v>144</v>
+      </c>
+      <c r="D33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" t="s">
+        <v>146</v>
+      </c>
+      <c r="F33" t="s">
+        <v>145</v>
+      </c>
+      <c r="G33" t="s">
+        <v>147</v>
+      </c>
+      <c r="H33" t="str">
+        <f>F33</f>
+        <v>Olorin</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" t="s">
+        <v>148</v>
+      </c>
+      <c r="D34" t="s">
+        <v>149</v>
+      </c>
+      <c r="E34" t="s">
+        <v>151</v>
+      </c>
+      <c r="F34" t="s">
+        <v>150</v>
+      </c>
+      <c r="G34" t="s">
+        <v>152</v>
+      </c>
+      <c r="H34" t="str">
+        <f>F34</f>
+        <v>Tak, tylko jeden</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" t="s">
+        <v>154</v>
+      </c>
+      <c r="D35" t="s">
+        <v>153</v>
+      </c>
+      <c r="E35" t="s">
+        <v>155</v>
+      </c>
+      <c r="F35" t="s">
+        <v>157</v>
+      </c>
+      <c r="G35" t="s">
+        <v>156</v>
+      </c>
+      <c r="H35" t="str">
+        <f>E35</f>
+        <v>Trzydziestu jeden Dunedainów, Gimli, Legolas oraz synowie Elronda</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" t="s">
+        <v>158</v>
+      </c>
+      <c r="D36" t="s">
+        <v>161</v>
+      </c>
+      <c r="E36" t="s">
+        <v>159</v>
+      </c>
+      <c r="F36" t="s">
+        <v>160</v>
+      </c>
+      <c r="G36" t="s">
+        <v>162</v>
+      </c>
+      <c r="H36" t="str">
+        <f>E36</f>
+        <v>Zguba Durina</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+      <c r="C37" t="s">
+        <v>163</v>
+      </c>
+      <c r="D37" t="s">
+        <v>164</v>
+      </c>
+      <c r="E37" t="s">
+        <v>165</v>
+      </c>
+      <c r="F37" t="s">
+        <v>166</v>
+      </c>
+      <c r="G37" t="s">
+        <v>167</v>
+      </c>
+      <c r="H37" t="str">
+        <f>E37</f>
+        <v>Quenya</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="C38" t="s">
+        <v>168</v>
+      </c>
+      <c r="D38" t="s">
+        <v>169</v>
+      </c>
+      <c r="E38" t="s">
+        <v>170</v>
+      </c>
+      <c r="F38" t="s">
+        <v>171</v>
+      </c>
+      <c r="G38" t="s">
+        <v>172</v>
+      </c>
+      <c r="H38" t="str">
+        <f>D38</f>
+        <v>Kili, Fili, Thorin</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>173</v>
+      </c>
+      <c r="C39" t="s">
+        <v>174</v>
+      </c>
+      <c r="D39" t="s">
+        <v>176</v>
+      </c>
+      <c r="E39" t="s">
+        <v>175</v>
+      </c>
+      <c r="F39" t="s">
+        <v>178</v>
+      </c>
+      <c r="G39" t="s">
+        <v>177</v>
+      </c>
+      <c r="H39" t="str">
+        <f>E39</f>
+        <v>Imladris</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" t="s">
+        <v>179</v>
+      </c>
+      <c r="D40" t="s">
+        <v>110</v>
+      </c>
+      <c r="E40" t="s">
+        <v>180</v>
+      </c>
+      <c r="F40" t="s">
+        <v>36</v>
+      </c>
+      <c r="G40" t="s">
+        <v>181</v>
+      </c>
+      <c r="H40" t="str">
+        <f>F40</f>
+        <v>Turin</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" t="s">
+        <v>182</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>3</v>
+      </c>
+      <c r="G41">
+        <v>4</v>
+      </c>
+      <c r="H41">
+        <f>2</f>
+        <v>2</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>130</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>